<commit_message>
Completed 1st term of ZB
Completed B
Completed K(without diploma)
Completed 1st term of ZB
</commit_message>
<xml_diff>
--- a/VIP_1_16_17.xlsx
+++ b/VIP_1_16_17.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/Documents/WORK/СЕКРЕТАР/НАВАНТАЖЕННЯ/VIPISKY/2016-2017/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/Documents/WORK/СЕКРЕТАР/НАВАНТАЖЕННЯ/VIPISKY/16-17/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Лист1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$1:$L$95</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$1:$L$100</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="161">
   <si>
     <t>Системи управління базами даних</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Управління інформаційно-телекомунікаційнми системами</t>
   </si>
   <si>
-    <t>Програмування -3.Системне програмування</t>
-  </si>
-  <si>
     <t>Компютеризовані системи управління-1. Промислові системи управління</t>
   </si>
   <si>
@@ -176,9 +173,6 @@
     <t>Писаренко А.В.</t>
   </si>
   <si>
-    <t>( тел. 454-92-25  )</t>
-  </si>
-  <si>
     <t>Програмування - 1. Алгоритмічне програмування</t>
   </si>
   <si>
@@ -200,9 +194,6 @@
     <t>Програмування -1. Алгоритмічне програмування</t>
   </si>
   <si>
-    <t>Інженерна та комп. графіка 1- Основи комп. графіки</t>
-  </si>
-  <si>
     <t>Операційні системи -1. Структура та функціонування ОС</t>
   </si>
   <si>
@@ -293,12 +284,6 @@
     <t xml:space="preserve">    </t>
   </si>
   <si>
-    <t>ІА-з41с</t>
-  </si>
-  <si>
-    <t>на 1 семестр 2015/2016 навчального року.</t>
-  </si>
-  <si>
     <t>Операційні системи - 1. Структура та функціонування ОС</t>
   </si>
   <si>
@@ -335,9 +320,6 @@
     <t>Оптимальнi системи керування - 1. Методи теорії оптимального керування</t>
   </si>
   <si>
-    <t>Сучасна теорія автоматичного управління - 1. Основи сучасної ТАУ</t>
-  </si>
-  <si>
     <t>Методи створення інформаційно-телекомунікаційних систем та мереж - 1. Проектування телекомунікаційних мереж та систем</t>
   </si>
   <si>
@@ -353,9 +335,6 @@
     <t>Сучасні технології створення програмних систем - 1. Технології забезпечення якості програмних систем</t>
   </si>
   <si>
-    <t>Управління інформаційно-телекомунікаційними системами</t>
-  </si>
-  <si>
     <t>Ас. Хмелюк М.С.</t>
   </si>
   <si>
@@ -383,21 +362,12 @@
     <t xml:space="preserve">Доц. Дорогий Я.Ю.           </t>
   </si>
   <si>
-    <t>Ст. викл.Долтна В.Г.</t>
-  </si>
-  <si>
     <t>Хмелюк М.С.</t>
   </si>
   <si>
-    <t>Ас. Март</t>
-  </si>
-  <si>
     <t xml:space="preserve">Доц. Катін П.Ю.      </t>
   </si>
   <si>
-    <t>ІА-з21</t>
-  </si>
-  <si>
     <t>Проектування компютеризованих систем управління -1. Програмно-технічні засоби проектування КСУ</t>
   </si>
   <si>
@@ -419,21 +389,9 @@
     <t>Ас. Галушко Д.О.</t>
   </si>
   <si>
-    <t>Ст. викл. Штифурик Ю.М.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ст. викл.Штифурик Ю.М. </t>
-  </si>
-  <si>
-    <t>NEW</t>
-  </si>
-  <si>
     <t>Безпека програм та даних</t>
   </si>
   <si>
-    <t>Доц. Полторак</t>
-  </si>
-  <si>
     <t>ІА-61,62</t>
   </si>
   <si>
@@ -449,9 +407,6 @@
     <t>ІА-з61</t>
   </si>
   <si>
-    <t xml:space="preserve">Проектування мікропроцесорних систем-1.Проектування МПС на базі мікроконтролерів родини  MCS-61    </t>
-  </si>
-  <si>
     <t>ІА-з61с</t>
   </si>
   <si>
@@ -479,9 +434,6 @@
     <t>Метрологія</t>
   </si>
   <si>
-    <t xml:space="preserve">Ст. викл. Штифурик Ю.М.  </t>
-  </si>
-  <si>
     <t>Комп'ютерна графіка</t>
   </si>
   <si>
@@ -525,6 +477,39 @@
   </si>
   <si>
     <t xml:space="preserve">31, - Ст. викл. Долина В.Г.                                    32,33 - Доц. Катін П.Ю.                                </t>
+  </si>
+  <si>
+    <t>Ст. викл. Штифурак Ю.М.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ст. викл. Штифурак Ю.М.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ст. викл.Штифурак Ю.М. </t>
+  </si>
+  <si>
+    <t>Комп. графіка</t>
+  </si>
+  <si>
+    <t>Математичне програмування та досл. операцій</t>
+  </si>
+  <si>
+    <t>Програмування -4. Системне програмування</t>
+  </si>
+  <si>
+    <t>ІА-з51</t>
+  </si>
+  <si>
+    <t>Комп'ютерна електроніка-2. Електроніка та мікросхемотехніка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Проектування мікропроцесорних систем-1.Проектування МПС на базі мікроконтролерів родини  MCS-51    </t>
+  </si>
+  <si>
+    <t>Надійність та діагностика</t>
+  </si>
+  <si>
+    <t>на 1 семестр 2016/2017 навчального року.</t>
   </si>
 </sst>
 </file>
@@ -588,7 +573,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -646,22 +631,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -783,9 +757,6 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1267,10 +1238,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:AB113"/>
+  <dimension ref="A2:AB117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="170" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="170" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1293,7 +1264,7 @@
   <sheetData>
     <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -1309,7 +1280,7 @@
     </row>
     <row r="3" spans="1:13" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -1325,7 +1296,7 @@
     </row>
     <row r="4" spans="1:13" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
@@ -1342,34 +1313,34 @@
     <row r="5" spans="1:13" ht="0.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="6" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="C6" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="D6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="E6" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="F6" s="19" t="s">
         <v>29</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>30</v>
       </c>
       <c r="G6" s="19"/>
       <c r="H6" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I6" s="19"/>
       <c r="J6" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K6" s="19"/>
       <c r="L6" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M6" s="20"/>
     </row>
@@ -1380,22 +1351,22 @@
       <c r="D7" s="17"/>
       <c r="E7" s="21"/>
       <c r="F7" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="22" t="s">
-        <v>35</v>
-      </c>
       <c r="H7" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="22" t="s">
-        <v>35</v>
-      </c>
       <c r="J7" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="22" t="s">
         <v>34</v>
-      </c>
-      <c r="K7" s="22" t="s">
-        <v>35</v>
       </c>
       <c r="L7" s="16"/>
       <c r="M7" s="23"/>
@@ -1405,19 +1376,19 @@
         <v>1</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="18">
         <v>1</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="G8" s="18">
         <v>2</v>
@@ -1425,7 +1396,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="18"/>
       <c r="J8" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K8" s="18">
         <v>2</v>
@@ -1443,13 +1414,13 @@
         <v>1</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G9" s="18">
         <v>1</v>
@@ -1457,7 +1428,7 @@
       <c r="H9" s="25"/>
       <c r="I9" s="18"/>
       <c r="J9" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K9" s="18">
         <v>1</v>
@@ -1475,13 +1446,13 @@
         <v>1</v>
       </c>
       <c r="D10" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>151</v>
-      </c>
       <c r="F10" s="25" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="G10" s="18">
         <v>2</v>
@@ -1489,7 +1460,7 @@
       <c r="H10" s="25"/>
       <c r="I10" s="18"/>
       <c r="J10" s="1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="K10" s="18">
         <v>1</v>
@@ -1507,13 +1478,13 @@
         <v>1</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G11" s="18">
         <v>1.5</v>
@@ -1521,7 +1492,7 @@
       <c r="H11" s="25"/>
       <c r="I11" s="18"/>
       <c r="J11" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="K11" s="18">
         <v>1.5</v>
@@ -1539,13 +1510,13 @@
         <v>1</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="G12" s="18">
         <v>1</v>
@@ -1553,7 +1524,7 @@
       <c r="H12" s="25"/>
       <c r="I12" s="18"/>
       <c r="J12" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="K12" s="18">
         <v>1</v>
@@ -1571,13 +1542,13 @@
         <v>1</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G13" s="18">
         <v>1.5</v>
@@ -1585,7 +1556,7 @@
       <c r="H13" s="25"/>
       <c r="I13" s="18"/>
       <c r="J13" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K13" s="18">
         <v>1.5</v>
@@ -1603,25 +1574,25 @@
         <v>1</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G14" s="18">
         <v>2</v>
       </c>
       <c r="H14" s="25" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I14" s="18">
         <v>2</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K14" s="18"/>
       <c r="L14" s="18"/>
@@ -1635,13 +1606,13 @@
         <v>1</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="G15" s="18">
         <v>2</v>
@@ -1649,7 +1620,7 @@
       <c r="H15" s="25"/>
       <c r="I15" s="18"/>
       <c r="J15" s="25" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="K15" s="18">
         <v>1.5</v>
@@ -1667,13 +1638,13 @@
         <v>2</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G16" s="18">
         <v>1.5</v>
@@ -1681,7 +1652,7 @@
       <c r="H16" s="25"/>
       <c r="I16" s="18"/>
       <c r="J16" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K16" s="18">
         <v>1.5</v>
@@ -1699,13 +1670,13 @@
         <v>2</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G17" s="18">
         <v>1</v>
@@ -1713,7 +1684,7 @@
       <c r="H17" s="25"/>
       <c r="I17" s="18"/>
       <c r="J17" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K17" s="18">
         <v>1</v>
@@ -1731,13 +1702,13 @@
         <v>2</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F18" s="25" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G18" s="18">
         <v>1</v>
@@ -1745,7 +1716,7 @@
       <c r="H18" s="25"/>
       <c r="I18" s="18"/>
       <c r="J18" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K18" s="18">
         <v>1</v>
@@ -1763,20 +1734,20 @@
         <v>2</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G19" s="18">
         <v>1.5</v>
       </c>
       <c r="H19" s="26"/>
       <c r="J19" s="27" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="K19" s="18">
         <v>1.5</v>
@@ -1794,13 +1765,13 @@
         <v>2</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G20" s="18">
         <v>2</v>
@@ -1808,7 +1779,7 @@
       <c r="H20" s="25"/>
       <c r="I20" s="25"/>
       <c r="J20" s="25" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="K20" s="18">
         <v>1</v>
@@ -1826,13 +1797,13 @@
         <v>3</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F21" s="25" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G21" s="18">
         <v>1.5</v>
@@ -1840,7 +1811,7 @@
       <c r="H21" s="25"/>
       <c r="I21" s="18"/>
       <c r="J21" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K21" s="18">
         <v>1</v>
@@ -1858,13 +1829,13 @@
         <v>3</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G22" s="18">
         <v>1.5</v>
@@ -1872,7 +1843,7 @@
       <c r="H22" s="25"/>
       <c r="I22" s="18"/>
       <c r="J22" s="1" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="K22" s="18">
         <v>1.5</v>
@@ -1890,13 +1861,13 @@
         <v>3</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G23" s="18">
         <v>1.5</v>
@@ -1904,7 +1875,7 @@
       <c r="H23" s="25"/>
       <c r="I23" s="18"/>
       <c r="J23" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="K23" s="18">
         <v>1</v>
@@ -1922,20 +1893,20 @@
         <v>3</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G24" s="18">
         <v>1.5</v>
       </c>
       <c r="I24" s="18"/>
       <c r="J24" s="25" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K24" s="18">
         <v>1</v>
@@ -1953,13 +1924,13 @@
         <v>3</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G25" s="18">
         <v>1</v>
@@ -1967,7 +1938,7 @@
       <c r="H25" s="25"/>
       <c r="I25" s="18"/>
       <c r="J25" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="K25" s="18">
         <v>1</v>
@@ -1985,13 +1956,13 @@
         <v>3</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G26" s="18">
         <v>1</v>
@@ -1999,7 +1970,7 @@
       <c r="H26" s="25"/>
       <c r="I26" s="18"/>
       <c r="J26" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K26" s="18">
         <v>1</v>
@@ -2017,13 +1988,13 @@
         <v>3</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="G27" s="18">
         <v>2</v>
@@ -2031,7 +2002,7 @@
       <c r="H27" s="25"/>
       <c r="I27" s="18"/>
       <c r="J27" s="25" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="K27" s="18">
         <v>1</v>
@@ -2049,13 +2020,13 @@
         <v>3</v>
       </c>
       <c r="D28" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="E28" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E28" s="9" t="s">
-        <v>96</v>
-      </c>
       <c r="F28" s="25" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="G28" s="18">
         <v>2</v>
@@ -2063,7 +2034,7 @@
       <c r="H28" s="25"/>
       <c r="I28" s="18"/>
       <c r="J28" s="1" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="K28" s="18">
         <v>1</v>
@@ -2081,13 +2052,13 @@
         <v>3</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G29" s="18">
         <v>1.5</v>
@@ -2095,7 +2066,7 @@
       <c r="H29" s="25"/>
       <c r="I29" s="18"/>
       <c r="J29" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K29" s="18">
         <v>1</v>
@@ -2113,13 +2084,13 @@
         <v>3</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F30" s="25" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="G30" s="18">
         <v>2</v>
@@ -2127,7 +2098,7 @@
       <c r="H30" s="25"/>
       <c r="I30" s="18"/>
       <c r="J30" s="25" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="K30" s="18">
         <v>1</v>
@@ -2145,13 +2116,13 @@
         <v>4</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" s="25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G31" s="18">
         <v>1</v>
@@ -2159,7 +2130,7 @@
       <c r="H31" s="25"/>
       <c r="I31" s="18"/>
       <c r="J31" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K31" s="18">
         <v>1</v>
@@ -2177,13 +2148,13 @@
         <v>4</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="F32" s="25" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G32" s="18">
         <v>1.5</v>
@@ -2191,7 +2162,7 @@
       <c r="H32" s="30"/>
       <c r="I32" s="18"/>
       <c r="J32" s="1" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="K32" s="18">
         <v>1</v>
@@ -2209,23 +2180,23 @@
         <v>4</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E33" s="31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" s="25" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G33" s="18">
         <v>1</v>
       </c>
       <c r="H33" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I33" s="18"/>
       <c r="J33" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="K33" s="18">
         <v>1</v>
@@ -2243,13 +2214,13 @@
         <v>4</v>
       </c>
       <c r="D34" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="32" t="s">
         <v>83</v>
-      </c>
-      <c r="E34" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34" s="32" t="s">
-        <v>86</v>
       </c>
       <c r="G34" s="18">
         <v>1.5</v>
@@ -2257,7 +2228,7 @@
       <c r="H34" s="25"/>
       <c r="I34" s="18"/>
       <c r="J34" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="K34" s="18">
         <v>1</v>
@@ -2275,13 +2246,13 @@
         <v>4</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E35" s="31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F35" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G35" s="18">
         <v>1.5</v>
@@ -2289,7 +2260,7 @@
       <c r="H35" s="25"/>
       <c r="I35" s="18"/>
       <c r="J35" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K35" s="18">
         <v>1.5</v>
@@ -2307,19 +2278,19 @@
         <v>4</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F36" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G36" s="18">
         <v>1</v>
       </c>
       <c r="H36" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I36" s="18">
         <v>1</v>
@@ -2337,13 +2308,13 @@
         <v>4</v>
       </c>
       <c r="D37" s="24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E37" s="31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F37" s="25" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G37" s="18">
         <v>1</v>
@@ -2351,7 +2322,7 @@
       <c r="H37" s="25"/>
       <c r="I37" s="18"/>
       <c r="J37" s="8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K37" s="18">
         <v>1</v>
@@ -2369,13 +2340,13 @@
         <v>4</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="F38" s="25" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G38" s="18">
         <v>2</v>
@@ -2383,7 +2354,7 @@
       <c r="H38" s="25"/>
       <c r="I38" s="18"/>
       <c r="J38" s="8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K38" s="18">
         <v>1</v>
@@ -2401,13 +2372,13 @@
         <v>4</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="F39" s="25" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G39" s="18">
         <v>2</v>
@@ -2415,7 +2386,7 @@
       <c r="H39" s="25"/>
       <c r="I39" s="18"/>
       <c r="J39" s="8" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="K39" s="18">
         <v>1</v>
@@ -2433,13 +2404,13 @@
         <v>4</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="F40" s="25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G40" s="18">
         <v>2</v>
@@ -2447,7 +2418,7 @@
       <c r="H40" s="25"/>
       <c r="I40" s="18"/>
       <c r="J40" s="8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="K40" s="18">
         <v>1</v>
@@ -2465,13 +2436,13 @@
         <v>4</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E41" s="29" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="F41" s="25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G41" s="18">
         <v>1.5</v>
@@ -2479,7 +2450,7 @@
       <c r="H41" s="25"/>
       <c r="I41" s="18"/>
       <c r="J41" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K41" s="18">
         <v>1</v>
@@ -2497,13 +2468,13 @@
         <v>1</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F42" s="25" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G42" s="18">
         <v>1</v>
@@ -2511,7 +2482,7 @@
       <c r="H42" s="25"/>
       <c r="I42" s="18"/>
       <c r="J42" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K42" s="18">
         <v>1</v>
@@ -2529,13 +2500,13 @@
         <v>1</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F43" s="25" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="G43" s="18">
         <v>1</v>
@@ -2543,7 +2514,7 @@
       <c r="H43" s="25"/>
       <c r="I43" s="18"/>
       <c r="J43" s="25" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="K43" s="18">
         <v>1</v>
@@ -2561,13 +2532,13 @@
         <v>1</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="F44" s="25" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G44" s="18">
         <v>2</v>
@@ -2575,7 +2546,7 @@
       <c r="H44" s="25"/>
       <c r="I44" s="18"/>
       <c r="J44" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K44" s="18">
         <v>1</v>
@@ -2593,13 +2564,13 @@
         <v>1</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F45" s="25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G45" s="18">
         <v>1</v>
@@ -2607,7 +2578,7 @@
       <c r="H45" s="25"/>
       <c r="I45" s="18"/>
       <c r="J45" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="K45" s="18">
         <v>1</v>
@@ -2625,25 +2596,25 @@
         <v>1</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F46" s="25" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G46" s="18">
         <v>1</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I46" s="18">
         <v>1</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K46" s="18">
         <v>1</v>
@@ -2661,13 +2632,13 @@
         <v>1</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F47" s="25" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G47" s="18">
         <v>1</v>
@@ -2675,7 +2646,7 @@
       <c r="H47" s="25"/>
       <c r="I47" s="18"/>
       <c r="J47" s="25" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K47" s="18">
         <v>1</v>
@@ -2693,19 +2664,19 @@
         <v>1</v>
       </c>
       <c r="D48" s="24" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F48" s="25" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G48" s="18">
         <v>1</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I48" s="18">
         <v>1</v>
@@ -2722,13 +2693,13 @@
         <v>1</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G49" s="18">
         <v>1</v>
@@ -2748,13 +2719,13 @@
         <v>1</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F50" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G50" s="18">
         <v>2</v>
@@ -2762,7 +2733,7 @@
       <c r="H50" s="25"/>
       <c r="I50" s="18"/>
       <c r="J50" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K50" s="18">
         <v>1</v>
@@ -2780,7 +2751,7 @@
         <v>1</v>
       </c>
       <c r="D51" s="24" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>6</v>
@@ -2788,7 +2759,7 @@
       <c r="G51" s="18"/>
       <c r="I51" s="18"/>
       <c r="J51" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K51" s="18">
         <v>1</v>
@@ -2806,19 +2777,19 @@
         <v>1</v>
       </c>
       <c r="D52" s="24" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G52" s="18">
         <v>0.5</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I52" s="18">
         <v>1</v>
@@ -2836,19 +2807,19 @@
         <v>1</v>
       </c>
       <c r="D53" s="24" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="F53" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G53" s="18">
         <v>0.5</v>
       </c>
       <c r="H53" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I53" s="18">
         <v>1</v>
@@ -2874,15 +2845,15 @@
     <row r="55" spans="1:13" s="34" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D55" s="35"/>
       <c r="E55" s="36" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F55" s="37"/>
       <c r="G55" s="35"/>
       <c r="H55" s="34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J55" s="37" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="K55" s="35"/>
     </row>
@@ -2902,7 +2873,7 @@
     </row>
     <row r="57" spans="1:13" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B57" s="10"/>
       <c r="C57" s="10"/>
@@ -2918,7 +2889,7 @@
     </row>
     <row r="58" spans="1:13" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B58" s="12"/>
       <c r="C58" s="12"/>
@@ -2934,7 +2905,7 @@
     </row>
     <row r="59" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" s="12" t="s">
-        <v>89</v>
+        <v>160</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
@@ -2953,34 +2924,34 @@
     </row>
     <row r="61" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B61" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C61" s="17" t="s">
+      <c r="D61" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D61" s="18" t="s">
+      <c r="E61" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E61" s="16" t="s">
+      <c r="F61" s="19" t="s">
         <v>29</v>
-      </c>
-      <c r="F61" s="19" t="s">
-        <v>30</v>
       </c>
       <c r="G61" s="19"/>
       <c r="H61" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I61" s="19"/>
       <c r="J61" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K61" s="19"/>
       <c r="L61" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M61" s="23"/>
     </row>
@@ -2991,22 +2962,22 @@
       <c r="D62" s="17"/>
       <c r="E62" s="16"/>
       <c r="F62" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="G62" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="G62" s="41" t="s">
-        <v>35</v>
-      </c>
       <c r="H62" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="I62" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="I62" s="41" t="s">
-        <v>35</v>
-      </c>
       <c r="J62" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="K62" s="41" t="s">
         <v>34</v>
-      </c>
-      <c r="K62" s="41" t="s">
-        <v>35</v>
       </c>
       <c r="L62" s="22"/>
     </row>
@@ -3015,30 +2986,30 @@
         <v>1</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C63" s="18">
         <v>1</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F63" s="25" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="G63" s="18">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="H63" s="25"/>
       <c r="I63" s="18"/>
       <c r="J63" s="25" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="K63" s="18">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="L63" s="18">
         <v>534</v>
@@ -3048,29 +3019,27 @@
       <c r="A64" s="18">
         <v>2</v>
       </c>
-      <c r="B64" s="18"/>
-      <c r="C64" s="18">
-        <v>1</v>
-      </c>
+      <c r="B64" s="16"/>
+      <c r="C64" s="18"/>
       <c r="D64" s="18" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F64" s="25" t="s">
-        <v>124</v>
+        <v>75</v>
       </c>
       <c r="G64" s="18">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H64" s="25"/>
       <c r="I64" s="18"/>
       <c r="J64" s="25" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="K64" s="18">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L64" s="18">
         <v>534</v>
@@ -3085,91 +3054,91 @@
         <v>1</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>58</v>
+        <v>153</v>
       </c>
       <c r="F65" s="25" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="G65" s="18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H65" s="25"/>
       <c r="I65" s="18"/>
       <c r="J65" s="25" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="K65" s="18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L65" s="18">
         <v>534</v>
       </c>
     </row>
-    <row r="66" spans="1:12" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:12" s="3" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="18">
         <v>4</v>
       </c>
       <c r="B66" s="18"/>
       <c r="C66" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="F66" s="25" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="G66" s="18">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H66" s="25"/>
       <c r="I66" s="18"/>
       <c r="J66" s="25" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="K66" s="18">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L66" s="18">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" s="3" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="18">
         <v>5</v>
       </c>
       <c r="B67" s="18"/>
       <c r="C67" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>42</v>
+        <v>134</v>
       </c>
       <c r="F67" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G67" s="18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H67" s="25"/>
       <c r="I67" s="18"/>
       <c r="J67" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K67" s="18">
         <v>2</v>
       </c>
       <c r="L67" s="18">
-        <v>617</v>
+        <v>517</v>
       </c>
     </row>
     <row r="68" spans="1:12" s="3" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3178,112 +3147,112 @@
       </c>
       <c r="B68" s="18"/>
       <c r="C68" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>59</v>
+        <v>154</v>
       </c>
       <c r="F68" s="25" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="G68" s="18">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H68" s="25"/>
       <c r="I68" s="18"/>
       <c r="J68" s="25" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="K68" s="18">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="L68" s="18">
         <v>534</v>
       </c>
     </row>
-    <row r="69" spans="1:12" s="3" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:12" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="18">
         <v>7</v>
       </c>
       <c r="B69" s="18"/>
       <c r="C69" s="18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D69" s="18" t="s">
-        <v>76</v>
+        <v>156</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>15</v>
+        <v>155</v>
       </c>
       <c r="F69" s="25" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="G69" s="18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H69" s="25"/>
       <c r="I69" s="18"/>
-      <c r="J69" s="1" t="s">
-        <v>62</v>
+      <c r="J69" s="25" t="s">
+        <v>79</v>
       </c>
       <c r="K69" s="18">
         <v>4</v>
       </c>
       <c r="L69" s="18">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" s="3" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="18">
         <v>8</v>
       </c>
       <c r="B70" s="18"/>
       <c r="C70" s="18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>76</v>
+        <v>156</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F70" s="25" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G70" s="18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H70" s="25"/>
       <c r="I70" s="18"/>
       <c r="J70" s="25" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="K70" s="18">
         <v>2</v>
       </c>
       <c r="L70" s="18">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" s="3" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" s="3" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="18">
         <v>9</v>
       </c>
       <c r="B71" s="18"/>
       <c r="C71" s="18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D71" s="18" t="s">
-        <v>76</v>
+        <v>156</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="F71" s="25" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="G71" s="18">
         <v>4</v>
@@ -3291,80 +3260,80 @@
       <c r="H71" s="25"/>
       <c r="I71" s="18"/>
       <c r="J71" s="25" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="K71" s="18">
         <v>4</v>
       </c>
       <c r="L71" s="18">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" s="3" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.15">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" s="3" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="18">
         <v>10</v>
       </c>
       <c r="B72" s="18"/>
       <c r="C72" s="18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D72" s="18" t="s">
-        <v>76</v>
+        <v>156</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="F72" s="25" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G72" s="18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H72" s="25"/>
       <c r="I72" s="18"/>
       <c r="J72" s="1" t="s">
-        <v>118</v>
+        <v>59</v>
       </c>
       <c r="K72" s="18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L72" s="18">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" s="3" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" s="3" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="18">
         <v>11</v>
       </c>
       <c r="B73" s="18"/>
       <c r="C73" s="18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D73" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>16</v>
+        <v>156</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="F73" s="25" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="G73" s="18">
         <v>4</v>
       </c>
       <c r="H73" s="25"/>
       <c r="I73" s="18"/>
-      <c r="J73" s="25" t="s">
-        <v>72</v>
+      <c r="J73" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="K73" s="18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L73" s="18">
         <v>534</v>
       </c>
     </row>
-    <row r="74" spans="1:12" s="3" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:12" s="3" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="18">
         <v>12</v>
       </c>
@@ -3373,26 +3342,27 @@
         <v>3</v>
       </c>
       <c r="D74" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="E74" s="9" t="s">
-        <v>52</v>
+        <v>95</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="F74" s="25" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="G74" s="18">
         <v>4</v>
       </c>
       <c r="H74" s="25"/>
-      <c r="J74" s="1" t="s">
-        <v>119</v>
+      <c r="I74" s="18"/>
+      <c r="J74" s="25" t="s">
+        <v>78</v>
       </c>
       <c r="K74" s="18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L74" s="18">
-        <v>534</v>
+        <v>309</v>
       </c>
     </row>
     <row r="75" spans="1:12" s="3" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3404,113 +3374,109 @@
         <v>3</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="E75" s="9" t="s">
-        <v>60</v>
+        <v>95</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="F75" s="25" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="G75" s="18">
         <v>6</v>
       </c>
-      <c r="H75" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="I75" s="18">
-        <v>4</v>
-      </c>
+      <c r="H75" s="25"/>
+      <c r="I75" s="18"/>
       <c r="J75" s="25" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="K75" s="18">
         <v>4</v>
       </c>
       <c r="L75" s="18">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" s="3" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" s="3" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="18">
         <v>14</v>
       </c>
       <c r="B76" s="18"/>
       <c r="C76" s="18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D76" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>22</v>
+        <v>95</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="F76" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="G76" s="42">
-        <v>2</v>
+        <v>60</v>
+      </c>
+      <c r="G76" s="18">
+        <v>4</v>
       </c>
       <c r="H76" s="25"/>
       <c r="I76" s="18"/>
       <c r="J76" s="25" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="K76" s="18">
-        <v>2</v>
-      </c>
-      <c r="L76" s="43">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" s="3" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>4</v>
+      </c>
+      <c r="L76" s="18">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" s="3" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="18">
         <v>15</v>
       </c>
       <c r="B77" s="18"/>
       <c r="C77" s="18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D77" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>0</v>
+        <v>95</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>157</v>
       </c>
       <c r="F77" s="25" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G77" s="18">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H77" s="25"/>
       <c r="I77" s="18"/>
-      <c r="J77" s="25" t="s">
-        <v>65</v>
+      <c r="J77" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="K77" s="18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L77" s="18">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" s="3" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" s="3" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="18">
         <v>16</v>
       </c>
       <c r="B78" s="18"/>
       <c r="C78" s="18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D78" s="18" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F78" s="25" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G78" s="18">
         <v>4</v>
@@ -3518,80 +3484,83 @@
       <c r="H78" s="25"/>
       <c r="I78" s="18"/>
       <c r="J78" s="25" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="K78" s="18">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L78" s="18">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" s="3" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.15">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" s="3" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="18">
         <v>17</v>
       </c>
       <c r="B79" s="18"/>
       <c r="C79" s="18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D79" s="18" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="F79" s="25" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="G79" s="18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H79" s="25"/>
-      <c r="I79" s="18"/>
-      <c r="J79" s="25" t="s">
-        <v>68</v>
+      <c r="J79" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="K79" s="18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L79" s="18">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" s="3" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" s="3" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="18">
         <v>18</v>
       </c>
       <c r="B80" s="18"/>
       <c r="C80" s="18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D80" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>3</v>
+        <v>95</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="F80" s="25" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="G80" s="18">
-        <v>4</v>
-      </c>
-      <c r="H80" s="25"/>
-      <c r="I80" s="18"/>
+        <v>6</v>
+      </c>
+      <c r="H80" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="I80" s="18">
+        <v>4</v>
+      </c>
       <c r="J80" s="25" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="K80" s="18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L80" s="18">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" s="3" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" s="3" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="18">
         <v>19</v>
       </c>
@@ -3600,30 +3569,30 @@
         <v>4</v>
       </c>
       <c r="D81" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="E81" s="9" t="s">
-        <v>140</v>
+        <v>73</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="F81" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="G81" s="18">
-        <v>4</v>
+        <v>79</v>
+      </c>
+      <c r="G81" s="42">
+        <v>2</v>
       </c>
       <c r="H81" s="25"/>
       <c r="I81" s="18"/>
-      <c r="J81" s="1" t="s">
-        <v>82</v>
+      <c r="J81" s="25" t="s">
+        <v>79</v>
       </c>
       <c r="K81" s="18">
         <v>2</v>
       </c>
-      <c r="L81" s="18">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" s="3" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L81" s="43">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" s="3" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="18">
         <v>20</v>
       </c>
@@ -3632,30 +3601,30 @@
         <v>4</v>
       </c>
       <c r="D82" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>10</v>
+        <v>73</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="F82" s="25" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="G82" s="18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H82" s="25"/>
       <c r="I82" s="18"/>
-      <c r="J82" s="1" t="s">
-        <v>120</v>
+      <c r="J82" s="25" t="s">
+        <v>62</v>
       </c>
       <c r="K82" s="18">
         <v>2</v>
       </c>
       <c r="L82" s="18">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" s="3" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" s="3" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="18">
         <v>21</v>
       </c>
@@ -3664,30 +3633,30 @@
         <v>4</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>122</v>
+        <v>73</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F83" s="25" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G83" s="18">
         <v>4</v>
       </c>
       <c r="H83" s="25"/>
       <c r="I83" s="18"/>
-      <c r="J83" s="1" t="s">
-        <v>62</v>
+      <c r="J83" s="25" t="s">
+        <v>63</v>
       </c>
       <c r="K83" s="18">
         <v>2</v>
       </c>
       <c r="L83" s="18">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" s="3" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.15">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" s="3" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="18">
         <v>22</v>
       </c>
@@ -3696,199 +3665,205 @@
         <v>4</v>
       </c>
       <c r="D84" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>4</v>
+        <v>73</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="F84" s="25" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G84" s="18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H84" s="25"/>
       <c r="I84" s="18"/>
       <c r="J84" s="25" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="K84" s="18">
         <v>2</v>
       </c>
       <c r="L84" s="18">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" s="3" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="18"/>
+        <v>309</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" s="3" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A85" s="18">
+        <v>23</v>
+      </c>
       <c r="B85" s="18"/>
       <c r="C85" s="18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D85" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="E85" s="9" t="s">
-        <v>103</v>
+        <v>73</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="F85" s="25" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="G85" s="18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H85" s="25"/>
       <c r="I85" s="18"/>
       <c r="J85" s="25" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="K85" s="18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L85" s="18">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" s="3" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A86" s="18"/>
+        <v>517</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" s="3" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A86" s="18">
+        <v>24</v>
+      </c>
       <c r="B86" s="18"/>
       <c r="C86" s="18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D86" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>101</v>
+        <v>73</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>158</v>
       </c>
       <c r="F86" s="25" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="G86" s="18">
-        <v>6</v>
-      </c>
-      <c r="H86" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="I86" s="18">
-        <v>4</v>
-      </c>
-      <c r="J86" s="25" t="s">
-        <v>69</v>
+        <v>4</v>
+      </c>
+      <c r="H86" s="25"/>
+      <c r="I86" s="18"/>
+      <c r="J86" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="K86" s="18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L86" s="18">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" s="3" customFormat="1" ht="83" customHeight="1" x14ac:dyDescent="0.15">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" s="3" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" s="18">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B87" s="18"/>
       <c r="C87" s="18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D87" s="18" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="E87" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>47</v>
+        <v>9</v>
+      </c>
+      <c r="F87" s="25" t="s">
+        <v>83</v>
       </c>
       <c r="G87" s="18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H87" s="25"/>
       <c r="I87" s="18"/>
-      <c r="J87" s="1"/>
-      <c r="K87" s="18"/>
-      <c r="L87" s="18"/>
+      <c r="J87" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K87" s="18">
+        <v>2</v>
+      </c>
+      <c r="L87" s="18">
+        <v>517</v>
+      </c>
     </row>
     <row r="88" spans="1:12" s="3" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="18">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B88" s="18"/>
       <c r="C88" s="18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D88" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="E88" s="9" t="s">
-        <v>105</v>
+        <v>73</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="F88" s="25" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G88" s="18">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H88" s="25"/>
       <c r="I88" s="18"/>
       <c r="J88" s="1" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="K88" s="18">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="L88" s="18">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" s="3" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" s="3" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="18">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B89" s="18"/>
       <c r="C89" s="18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D89" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="E89" s="9" t="s">
-        <v>123</v>
+        <v>73</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="F89" s="25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G89" s="18">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H89" s="25"/>
       <c r="I89" s="18"/>
-      <c r="J89" s="1" t="s">
-        <v>68</v>
+      <c r="J89" s="25" t="s">
+        <v>66</v>
       </c>
       <c r="K89" s="18">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L89" s="18">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" s="3" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" s="3" customFormat="1" ht="91" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="18">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B90" s="18"/>
       <c r="C90" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D90" s="18" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F90" s="25" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="G90" s="18">
         <v>6</v>
@@ -3896,406 +3871,460 @@
       <c r="H90" s="25"/>
       <c r="I90" s="18"/>
       <c r="J90" s="25" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="K90" s="18">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L90" s="18">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" s="3" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" s="3" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="18">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B91" s="18"/>
       <c r="C91" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D91" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="E91" s="9" t="s">
-        <v>107</v>
+        <v>126</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="F91" s="25" t="s">
-        <v>124</v>
+        <v>66</v>
       </c>
       <c r="G91" s="18">
         <v>6</v>
       </c>
-      <c r="H91" s="25"/>
-      <c r="I91" s="18"/>
+      <c r="H91" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="I91" s="18">
+        <v>4</v>
+      </c>
       <c r="J91" s="25" t="s">
-        <v>124</v>
+        <v>66</v>
       </c>
       <c r="K91" s="18">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L91" s="18">
         <v>534</v>
       </c>
     </row>
-    <row r="92" spans="1:12" s="3" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:12" s="3" customFormat="1" ht="83" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92" s="18">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B92" s="18"/>
       <c r="C92" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D92" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="E92" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="F92" s="25" t="s">
-        <v>68</v>
+        <v>126</v>
+      </c>
+      <c r="E92" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="G92" s="18">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H92" s="25"/>
       <c r="I92" s="18"/>
-      <c r="J92" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="K92" s="18">
-        <v>4</v>
-      </c>
-      <c r="L92" s="18">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" s="33" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="J92" s="1"/>
+      <c r="K92" s="18"/>
+      <c r="L92" s="18"/>
+    </row>
+    <row r="93" spans="1:12" s="3" customFormat="1" ht="94" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="18">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B93" s="18"/>
       <c r="C93" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D93" s="18" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="E93" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F93" s="25"/>
-      <c r="G93" s="18"/>
-      <c r="H93" s="44" t="s">
-        <v>80</v>
-      </c>
-      <c r="I93" s="18">
+        <v>99</v>
+      </c>
+      <c r="F93" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="G93" s="18">
+        <v>8</v>
+      </c>
+      <c r="H93" s="25"/>
+      <c r="I93" s="18"/>
+      <c r="J93" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K93" s="18">
+        <v>8</v>
+      </c>
+      <c r="L93" s="18">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" s="3" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A94" s="18">
+        <v>32</v>
+      </c>
+      <c r="B94" s="18"/>
+      <c r="C94" s="18">
+        <v>5</v>
+      </c>
+      <c r="D94" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E94" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F94" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="G94" s="18">
+        <v>10</v>
+      </c>
+      <c r="H94" s="25"/>
+      <c r="I94" s="18"/>
+      <c r="J94" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K94" s="18">
         <v>6</v>
       </c>
-      <c r="J93" s="25"/>
-      <c r="K93" s="18"/>
-      <c r="L93" s="18"/>
-    </row>
-    <row r="94" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A94" s="35"/>
-      <c r="B94" s="35"/>
-      <c r="C94" s="35"/>
-      <c r="D94" s="35"/>
-      <c r="E94" s="45"/>
-      <c r="F94" s="46"/>
-      <c r="G94" s="35"/>
-      <c r="H94" s="46"/>
-      <c r="I94" s="35"/>
-      <c r="J94" s="47"/>
-      <c r="K94" s="35"/>
-      <c r="L94" s="35"/>
-    </row>
-    <row r="95" spans="1:12" s="51" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="48"/>
-      <c r="B95" s="48"/>
-      <c r="C95" s="49"/>
-      <c r="D95" s="33"/>
-      <c r="E95" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F95" s="11"/>
-      <c r="G95" s="50"/>
-      <c r="H95" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="I95" s="34"/>
-      <c r="J95" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="K95" s="48"/>
-      <c r="L95" s="33"/>
-    </row>
-    <row r="96" spans="1:12" s="51" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A96" s="50"/>
-      <c r="B96" s="50"/>
-      <c r="C96" s="11"/>
-      <c r="D96" s="52"/>
-      <c r="E96" s="53" t="s">
-        <v>132</v>
-      </c>
-      <c r="F96" s="54"/>
-      <c r="G96" s="50"/>
-      <c r="H96" s="55"/>
-      <c r="I96" s="11"/>
-      <c r="J96" s="54"/>
-      <c r="K96" s="50"/>
-    </row>
-    <row r="97" spans="1:28" s="51" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A97" s="50"/>
-      <c r="B97" s="50"/>
-      <c r="C97" s="50"/>
-      <c r="D97" s="54"/>
-      <c r="E97" s="67"/>
-      <c r="F97" s="68"/>
-      <c r="G97" s="68"/>
-      <c r="H97" s="56"/>
-      <c r="I97" s="57"/>
-      <c r="J97" s="58"/>
-      <c r="K97" s="50"/>
-    </row>
-    <row r="98" spans="1:28" s="51" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="L94" s="18">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" s="3" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A95" s="18">
+        <v>33</v>
+      </c>
+      <c r="B95" s="18"/>
+      <c r="C95" s="18">
+        <v>5</v>
+      </c>
+      <c r="D95" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E95" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="F95" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="G95" s="18">
+        <v>6</v>
+      </c>
+      <c r="H95" s="25"/>
+      <c r="I95" s="18"/>
+      <c r="J95" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="K95" s="18">
+        <v>6</v>
+      </c>
+      <c r="L95" s="18">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" s="3" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A96" s="18">
+        <v>34</v>
+      </c>
+      <c r="B96" s="18"/>
+      <c r="C96" s="18">
+        <v>5</v>
+      </c>
+      <c r="D96" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E96" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F96" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="G96" s="18">
+        <v>6</v>
+      </c>
+      <c r="H96" s="25"/>
+      <c r="I96" s="18"/>
+      <c r="J96" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="K96" s="18">
+        <v>6</v>
+      </c>
+      <c r="L96" s="18">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="97" spans="1:28" s="3" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A97" s="18">
+        <v>35</v>
+      </c>
+      <c r="B97" s="18"/>
+      <c r="C97" s="18">
+        <v>5</v>
+      </c>
+      <c r="D97" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E97" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="F97" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="G97" s="18">
+        <v>4</v>
+      </c>
+      <c r="H97" s="25"/>
+      <c r="I97" s="18"/>
+      <c r="J97" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="K97" s="18">
+        <v>4</v>
+      </c>
+      <c r="L97" s="18">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="98" spans="1:28" s="3" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A98" s="18">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B98" s="18"/>
       <c r="C98" s="18">
-        <v>7</v>
-      </c>
-      <c r="D98" s="18"/>
-      <c r="E98" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="F98" s="25"/>
-      <c r="G98" s="18"/>
-      <c r="H98" s="44" t="s">
-        <v>134</v>
-      </c>
-      <c r="I98" s="18"/>
+        <v>5</v>
+      </c>
+      <c r="D98" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E98" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="F98" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="G98" s="18">
+        <v>4</v>
+      </c>
+      <c r="H98" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="I98" s="18">
+        <v>2</v>
+      </c>
       <c r="J98" s="25"/>
       <c r="K98" s="18"/>
       <c r="L98" s="18"/>
-      <c r="M98" s="62"/>
-      <c r="N98" s="62"/>
-      <c r="O98" s="62"/>
-      <c r="P98" s="62"/>
-      <c r="Q98" s="62"/>
-      <c r="R98" s="62"/>
-      <c r="S98" s="62"/>
-      <c r="T98" s="62"/>
-      <c r="U98" s="62"/>
-      <c r="V98" s="62"/>
-      <c r="W98" s="62"/>
-      <c r="X98" s="62"/>
-      <c r="Y98" s="62"/>
-      <c r="Z98" s="62"/>
-      <c r="AA98" s="62"/>
-      <c r="AB98" s="62"/>
-    </row>
-    <row r="99" spans="1:28" s="51" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A99" s="50"/>
-      <c r="B99" s="59"/>
-      <c r="C99" s="59"/>
-      <c r="D99" s="60"/>
-      <c r="E99" s="61"/>
-      <c r="F99" s="69"/>
-      <c r="G99" s="70"/>
-      <c r="H99" s="62"/>
-      <c r="I99" s="62"/>
-      <c r="J99" s="62"/>
-      <c r="K99" s="59"/>
-      <c r="L99" s="62"/>
-      <c r="M99" s="62"/>
-      <c r="N99" s="62"/>
-      <c r="O99" s="62"/>
-      <c r="P99" s="62"/>
-      <c r="Q99" s="62"/>
-      <c r="R99" s="62"/>
-      <c r="S99" s="62"/>
-      <c r="T99" s="62"/>
-      <c r="U99" s="62"/>
-      <c r="V99" s="62"/>
-      <c r="W99" s="62"/>
-      <c r="X99" s="62"/>
-      <c r="Y99" s="62"/>
-      <c r="Z99" s="62"/>
-      <c r="AA99" s="62"/>
-      <c r="AB99" s="62"/>
-    </row>
-    <row r="100" spans="1:28" s="51" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A100" s="50"/>
-      <c r="B100" s="59"/>
-      <c r="C100" s="59"/>
-      <c r="D100" s="60"/>
-      <c r="E100" s="61"/>
-      <c r="F100" s="60"/>
-      <c r="G100" s="59"/>
-      <c r="H100" s="61"/>
-      <c r="I100" s="63"/>
-      <c r="J100" s="60"/>
-      <c r="K100" s="59"/>
-      <c r="L100" s="62"/>
-      <c r="M100" s="62"/>
-      <c r="N100" s="62"/>
-      <c r="O100" s="62"/>
-      <c r="P100" s="62"/>
-      <c r="Q100" s="62"/>
-      <c r="R100" s="62"/>
-      <c r="S100" s="62"/>
-      <c r="T100" s="62"/>
-      <c r="U100" s="62"/>
-      <c r="V100" s="62"/>
-      <c r="W100" s="62"/>
-      <c r="X100" s="62"/>
-      <c r="Y100" s="62"/>
-      <c r="Z100" s="62"/>
-      <c r="AA100" s="62"/>
-      <c r="AB100" s="62"/>
-    </row>
-    <row r="101" spans="1:28" s="51" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A101" s="50"/>
-      <c r="B101" s="59"/>
-      <c r="C101" s="59"/>
-      <c r="D101" s="60"/>
-      <c r="E101" s="61"/>
-      <c r="F101" s="60"/>
-      <c r="G101" s="59"/>
-      <c r="H101" s="62"/>
-      <c r="I101" s="62"/>
-      <c r="J101" s="62"/>
-      <c r="K101" s="59"/>
-      <c r="L101" s="62"/>
-      <c r="M101" s="62"/>
-      <c r="N101" s="62"/>
-      <c r="O101" s="62"/>
-      <c r="P101" s="62"/>
-      <c r="Q101" s="62"/>
-      <c r="R101" s="62"/>
-      <c r="S101" s="62"/>
-      <c r="T101" s="62"/>
-      <c r="U101" s="62"/>
-      <c r="V101" s="62"/>
-      <c r="W101" s="62"/>
-      <c r="X101" s="62"/>
-      <c r="Y101" s="62"/>
-      <c r="Z101" s="62"/>
-      <c r="AA101" s="62"/>
-      <c r="AB101" s="62"/>
-    </row>
-    <row r="102" spans="1:28" s="51" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A102" s="50"/>
-      <c r="B102" s="59"/>
-      <c r="C102" s="59"/>
-      <c r="D102" s="60"/>
-      <c r="E102" s="61"/>
-      <c r="F102" s="60"/>
-      <c r="G102" s="59"/>
-      <c r="H102" s="62"/>
-      <c r="I102" s="62"/>
-      <c r="J102" s="62"/>
-      <c r="K102" s="59"/>
-      <c r="L102" s="62"/>
-      <c r="M102" s="62"/>
-      <c r="N102" s="62"/>
-      <c r="O102" s="62"/>
-      <c r="P102" s="62"/>
-      <c r="Q102" s="62"/>
-      <c r="R102" s="62"/>
-      <c r="S102" s="62"/>
-      <c r="T102" s="62"/>
-      <c r="U102" s="62"/>
-      <c r="V102" s="62"/>
-      <c r="W102" s="62"/>
-      <c r="X102" s="62"/>
-      <c r="Y102" s="62"/>
-      <c r="Z102" s="62"/>
-      <c r="AA102" s="62"/>
-      <c r="AB102" s="62"/>
-    </row>
-    <row r="103" spans="1:28" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="59"/>
-      <c r="B103" s="59"/>
-      <c r="C103" s="59"/>
-      <c r="D103" s="60"/>
-      <c r="E103" s="61"/>
-      <c r="F103" s="60"/>
-      <c r="G103" s="62"/>
-      <c r="H103" s="34"/>
-      <c r="I103" s="34"/>
-      <c r="J103" s="37"/>
-      <c r="K103" s="59"/>
-      <c r="L103" s="62"/>
-      <c r="M103" s="64"/>
-      <c r="N103" s="64"/>
-      <c r="O103" s="64"/>
-      <c r="P103" s="64"/>
-      <c r="Q103" s="64"/>
-      <c r="R103" s="64"/>
-      <c r="S103" s="64"/>
-      <c r="T103" s="64"/>
-      <c r="U103" s="64"/>
-      <c r="V103" s="64"/>
-      <c r="W103" s="64"/>
-      <c r="X103" s="64"/>
-      <c r="Y103" s="64"/>
-      <c r="Z103" s="64"/>
-      <c r="AA103" s="64"/>
-      <c r="AB103" s="64"/>
-    </row>
-    <row r="104" spans="1:28" s="63" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A104" s="59"/>
-      <c r="B104" s="59"/>
-      <c r="C104" s="59"/>
-      <c r="D104" s="60"/>
-      <c r="E104" s="62"/>
-      <c r="F104" s="62"/>
-      <c r="G104" s="62"/>
-      <c r="H104" s="62"/>
+    </row>
+    <row r="99" spans="1:28" s="50" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A99" s="35"/>
+      <c r="B99" s="35"/>
+      <c r="C99" s="35"/>
+      <c r="D99" s="35"/>
+      <c r="E99" s="44"/>
+      <c r="F99" s="45"/>
+      <c r="G99" s="35"/>
+      <c r="H99" s="45"/>
+      <c r="I99" s="35"/>
+      <c r="J99" s="46"/>
+      <c r="K99" s="35"/>
+      <c r="L99" s="35"/>
+    </row>
+    <row r="100" spans="1:28" s="50" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="47"/>
+      <c r="B100" s="47"/>
+      <c r="C100" s="48"/>
+      <c r="D100" s="33"/>
+      <c r="E100" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F100" s="11"/>
+      <c r="G100" s="49"/>
+      <c r="H100" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="I100" s="34"/>
+      <c r="J100" s="37" t="s">
+        <v>147</v>
+      </c>
+      <c r="K100" s="47"/>
+      <c r="L100" s="33"/>
+    </row>
+    <row r="101" spans="1:28" s="50" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A101" s="49"/>
+      <c r="B101" s="49"/>
+      <c r="C101" s="11"/>
+      <c r="D101" s="51"/>
+      <c r="E101" s="52"/>
+      <c r="F101" s="53"/>
+      <c r="G101" s="49"/>
+      <c r="H101" s="54"/>
+      <c r="I101" s="11"/>
+      <c r="J101" s="53"/>
+      <c r="K101" s="49"/>
+    </row>
+    <row r="102" spans="1:28" s="50" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A102" s="49"/>
+      <c r="B102" s="49"/>
+      <c r="C102" s="49"/>
+      <c r="D102" s="53"/>
+      <c r="E102" s="66"/>
+      <c r="F102" s="67"/>
+      <c r="G102" s="67"/>
+      <c r="H102" s="55"/>
+      <c r="I102" s="56"/>
+      <c r="J102" s="57"/>
+      <c r="K102" s="49"/>
+    </row>
+    <row r="103" spans="1:28" s="50" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A103" s="49"/>
+      <c r="B103" s="58"/>
+      <c r="C103" s="58"/>
+      <c r="D103" s="59"/>
+      <c r="E103" s="60"/>
+      <c r="F103" s="68"/>
+      <c r="G103" s="69"/>
+      <c r="H103" s="61"/>
+      <c r="I103" s="61"/>
+      <c r="J103" s="61"/>
+      <c r="K103" s="58"/>
+      <c r="L103" s="61"/>
+      <c r="M103" s="61"/>
+      <c r="N103" s="61"/>
+      <c r="O103" s="61"/>
+      <c r="P103" s="61"/>
+      <c r="Q103" s="61"/>
+      <c r="R103" s="61"/>
+      <c r="S103" s="61"/>
+      <c r="T103" s="61"/>
+      <c r="U103" s="61"/>
+      <c r="V103" s="61"/>
+      <c r="W103" s="61"/>
+      <c r="X103" s="61"/>
+      <c r="Y103" s="61"/>
+      <c r="Z103" s="61"/>
+      <c r="AA103" s="61"/>
+      <c r="AB103" s="61"/>
+    </row>
+    <row r="104" spans="1:28" s="50" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A104" s="49"/>
+      <c r="B104" s="58"/>
+      <c r="C104" s="58"/>
+      <c r="D104" s="59"/>
+      <c r="E104" s="60"/>
+      <c r="F104" s="59"/>
+      <c r="G104" s="58"/>
+      <c r="H104" s="60"/>
       <c r="I104" s="62"/>
-      <c r="J104" s="62"/>
-      <c r="K104" s="59"/>
-      <c r="L104" s="62"/>
-    </row>
-    <row r="105" spans="1:28" s="63" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A105" s="5"/>
-      <c r="B105" s="5"/>
-      <c r="C105" s="5"/>
-      <c r="D105" s="5"/>
-      <c r="E105" s="5"/>
-      <c r="F105" s="5"/>
-      <c r="G105" s="5"/>
-      <c r="H105" s="5"/>
-      <c r="I105" s="5"/>
-      <c r="J105" s="5"/>
-      <c r="K105" s="5"/>
-      <c r="L105" s="5"/>
-    </row>
-    <row r="106" spans="1:28" s="63" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A106" s="65"/>
-      <c r="B106" s="65"/>
-      <c r="C106" s="65"/>
-      <c r="D106" s="65"/>
-      <c r="E106" s="66"/>
-      <c r="G106" s="65"/>
-      <c r="I106" s="65"/>
-      <c r="K106" s="65"/>
-    </row>
-    <row r="107" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A107" s="65"/>
-      <c r="B107" s="65"/>
-      <c r="C107" s="65"/>
-      <c r="D107" s="65"/>
-      <c r="E107" s="66"/>
-      <c r="F107" s="63"/>
-      <c r="G107" s="65"/>
-      <c r="H107" s="63"/>
-      <c r="I107" s="65"/>
-      <c r="J107" s="63"/>
-      <c r="K107" s="65"/>
-      <c r="L107" s="63"/>
+      <c r="J104" s="59"/>
+      <c r="K104" s="58"/>
+      <c r="L104" s="61"/>
+      <c r="M104" s="61"/>
+      <c r="N104" s="61"/>
+      <c r="O104" s="61"/>
+      <c r="P104" s="61"/>
+      <c r="Q104" s="61"/>
+      <c r="R104" s="61"/>
+      <c r="S104" s="61"/>
+      <c r="T104" s="61"/>
+      <c r="U104" s="61"/>
+      <c r="V104" s="61"/>
+      <c r="W104" s="61"/>
+      <c r="X104" s="61"/>
+      <c r="Y104" s="61"/>
+      <c r="Z104" s="61"/>
+      <c r="AA104" s="61"/>
+      <c r="AB104" s="61"/>
+    </row>
+    <row r="105" spans="1:28" s="50" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A105" s="49"/>
+      <c r="B105" s="58"/>
+      <c r="C105" s="58"/>
+      <c r="D105" s="59"/>
+      <c r="E105" s="60"/>
+      <c r="F105" s="59"/>
+      <c r="G105" s="58"/>
+      <c r="H105" s="61"/>
+      <c r="I105" s="61"/>
+      <c r="J105" s="61"/>
+      <c r="K105" s="58"/>
+      <c r="L105" s="61"/>
+      <c r="M105" s="61"/>
+      <c r="N105" s="61"/>
+      <c r="O105" s="61"/>
+      <c r="P105" s="61"/>
+      <c r="Q105" s="61"/>
+      <c r="R105" s="61"/>
+      <c r="S105" s="61"/>
+      <c r="T105" s="61"/>
+      <c r="U105" s="61"/>
+      <c r="V105" s="61"/>
+      <c r="W105" s="61"/>
+      <c r="X105" s="61"/>
+      <c r="Y105" s="61"/>
+      <c r="Z105" s="61"/>
+      <c r="AA105" s="61"/>
+      <c r="AB105" s="61"/>
+    </row>
+    <row r="106" spans="1:28" s="50" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A106" s="49"/>
+      <c r="B106" s="58"/>
+      <c r="C106" s="58"/>
+      <c r="D106" s="59"/>
+      <c r="E106" s="60"/>
+      <c r="F106" s="59"/>
+      <c r="G106" s="58"/>
+      <c r="H106" s="61"/>
+      <c r="I106" s="61"/>
+      <c r="J106" s="61"/>
+      <c r="K106" s="58"/>
+      <c r="L106" s="61"/>
+      <c r="M106" s="61"/>
+      <c r="N106" s="61"/>
+      <c r="O106" s="61"/>
+      <c r="P106" s="61"/>
+      <c r="Q106" s="61"/>
+      <c r="R106" s="61"/>
+      <c r="S106" s="61"/>
+      <c r="T106" s="61"/>
+      <c r="U106" s="61"/>
+      <c r="V106" s="61"/>
+      <c r="W106" s="61"/>
+      <c r="X106" s="61"/>
+      <c r="Y106" s="61"/>
+      <c r="Z106" s="61"/>
+      <c r="AA106" s="61"/>
+      <c r="AB106" s="61"/>
+    </row>
+    <row r="107" spans="1:28" s="33" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="58"/>
+      <c r="B107" s="58"/>
+      <c r="C107" s="58"/>
+      <c r="D107" s="59"/>
+      <c r="E107" s="60"/>
+      <c r="F107" s="59"/>
+      <c r="G107" s="61"/>
+      <c r="H107" s="34"/>
+      <c r="I107" s="34"/>
+      <c r="J107" s="37"/>
+      <c r="K107" s="58"/>
+      <c r="L107" s="61"/>
       <c r="M107" s="63"/>
       <c r="N107" s="63"/>
       <c r="O107" s="63"/>
@@ -4313,169 +4342,237 @@
       <c r="AA107" s="63"/>
       <c r="AB107" s="63"/>
     </row>
-    <row r="108" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A108" s="65"/>
-      <c r="B108" s="65"/>
-      <c r="C108" s="65"/>
-      <c r="D108" s="65"/>
-      <c r="E108" s="66"/>
-      <c r="F108" s="63"/>
-      <c r="G108" s="65"/>
-      <c r="H108" s="63"/>
-      <c r="I108" s="65"/>
-      <c r="J108" s="63"/>
-      <c r="K108" s="65"/>
-      <c r="L108" s="63"/>
-      <c r="M108" s="63"/>
-      <c r="N108" s="63"/>
-      <c r="O108" s="63"/>
-      <c r="P108" s="63"/>
-      <c r="Q108" s="63"/>
-      <c r="R108" s="63"/>
-      <c r="S108" s="63"/>
-      <c r="T108" s="63"/>
-      <c r="U108" s="63"/>
-      <c r="V108" s="63"/>
-      <c r="W108" s="63"/>
-      <c r="X108" s="63"/>
-      <c r="Y108" s="63"/>
-      <c r="Z108" s="63"/>
-      <c r="AA108" s="63"/>
-      <c r="AB108" s="63"/>
-    </row>
-    <row r="109" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="B109" s="65"/>
-      <c r="C109" s="65"/>
-      <c r="D109" s="65"/>
-      <c r="E109" s="66"/>
-      <c r="F109" s="63"/>
-      <c r="G109" s="65"/>
-      <c r="H109" s="63"/>
-      <c r="I109" s="65"/>
-      <c r="J109" s="63"/>
-      <c r="K109" s="65"/>
-      <c r="L109" s="63"/>
-      <c r="M109" s="63"/>
-      <c r="N109" s="63"/>
-      <c r="O109" s="63"/>
-      <c r="P109" s="63"/>
-      <c r="Q109" s="63"/>
-      <c r="R109" s="63"/>
-      <c r="S109" s="63"/>
-      <c r="T109" s="63"/>
-      <c r="U109" s="63"/>
-      <c r="V109" s="63"/>
-      <c r="W109" s="63"/>
-      <c r="X109" s="63"/>
-      <c r="Y109" s="63"/>
-      <c r="Z109" s="63"/>
-      <c r="AA109" s="63"/>
-      <c r="AB109" s="63"/>
-    </row>
-    <row r="110" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="B110" s="65"/>
-      <c r="C110" s="65"/>
-      <c r="D110" s="65"/>
-      <c r="E110" s="66"/>
-      <c r="F110" s="63"/>
-      <c r="G110" s="65"/>
-      <c r="H110" s="63"/>
-      <c r="I110" s="65"/>
-      <c r="J110" s="63"/>
-      <c r="K110" s="65"/>
-      <c r="L110" s="63"/>
-      <c r="M110" s="63"/>
-      <c r="N110" s="63"/>
-      <c r="O110" s="63"/>
-      <c r="P110" s="63"/>
-      <c r="Q110" s="63"/>
-      <c r="R110" s="63"/>
-      <c r="S110" s="63"/>
-      <c r="T110" s="63"/>
-      <c r="U110" s="63"/>
-      <c r="V110" s="63"/>
-      <c r="W110" s="63"/>
-      <c r="X110" s="63"/>
-      <c r="Y110" s="63"/>
-      <c r="Z110" s="63"/>
-      <c r="AA110" s="63"/>
-      <c r="AB110" s="63"/>
+    <row r="108" spans="1:28" s="62" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A108" s="58"/>
+      <c r="B108" s="58"/>
+      <c r="C108" s="58"/>
+      <c r="D108" s="59"/>
+      <c r="E108" s="61"/>
+      <c r="F108" s="61"/>
+      <c r="G108" s="61"/>
+      <c r="H108" s="61"/>
+      <c r="I108" s="61"/>
+      <c r="J108" s="61"/>
+      <c r="K108" s="58"/>
+      <c r="L108" s="61"/>
+    </row>
+    <row r="109" spans="1:28" s="62" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A109" s="5"/>
+      <c r="B109" s="5"/>
+      <c r="C109" s="5"/>
+      <c r="D109" s="5"/>
+      <c r="E109" s="5"/>
+      <c r="F109" s="5"/>
+      <c r="G109" s="5"/>
+      <c r="H109" s="5"/>
+      <c r="I109" s="5"/>
+      <c r="J109" s="5"/>
+      <c r="K109" s="5"/>
+      <c r="L109" s="5"/>
+    </row>
+    <row r="110" spans="1:28" s="62" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A110" s="64"/>
+      <c r="B110" s="64"/>
+      <c r="C110" s="64"/>
+      <c r="D110" s="64"/>
+      <c r="E110" s="65"/>
+      <c r="G110" s="64"/>
+      <c r="I110" s="64"/>
+      <c r="K110" s="64"/>
     </row>
     <row r="111" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="B111" s="65"/>
-      <c r="C111" s="65"/>
-      <c r="D111" s="65"/>
-      <c r="E111" s="66"/>
-      <c r="F111" s="63"/>
-      <c r="G111" s="65"/>
-      <c r="H111" s="63"/>
-      <c r="I111" s="65"/>
-      <c r="J111" s="63"/>
-      <c r="K111" s="65"/>
-      <c r="L111" s="63"/>
-      <c r="M111" s="63"/>
-      <c r="N111" s="63"/>
-      <c r="O111" s="63"/>
-      <c r="P111" s="63"/>
-      <c r="Q111" s="63"/>
-      <c r="R111" s="63"/>
-      <c r="S111" s="63"/>
-      <c r="T111" s="63"/>
-      <c r="U111" s="63"/>
-      <c r="V111" s="63"/>
-      <c r="W111" s="63"/>
-      <c r="X111" s="63"/>
-      <c r="Y111" s="63"/>
-      <c r="Z111" s="63"/>
-      <c r="AA111" s="63"/>
-      <c r="AB111" s="63"/>
+      <c r="A111" s="64"/>
+      <c r="B111" s="64"/>
+      <c r="C111" s="64"/>
+      <c r="D111" s="64"/>
+      <c r="E111" s="65"/>
+      <c r="F111" s="62"/>
+      <c r="G111" s="64"/>
+      <c r="H111" s="62"/>
+      <c r="I111" s="64"/>
+      <c r="J111" s="62"/>
+      <c r="K111" s="64"/>
+      <c r="L111" s="62"/>
+      <c r="M111" s="62"/>
+      <c r="N111" s="62"/>
+      <c r="O111" s="62"/>
+      <c r="P111" s="62"/>
+      <c r="Q111" s="62"/>
+      <c r="R111" s="62"/>
+      <c r="S111" s="62"/>
+      <c r="T111" s="62"/>
+      <c r="U111" s="62"/>
+      <c r="V111" s="62"/>
+      <c r="W111" s="62"/>
+      <c r="X111" s="62"/>
+      <c r="Y111" s="62"/>
+      <c r="Z111" s="62"/>
+      <c r="AA111" s="62"/>
+      <c r="AB111" s="62"/>
     </row>
     <row r="112" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="B112" s="65"/>
-      <c r="C112" s="65"/>
-      <c r="D112" s="65"/>
-      <c r="E112" s="66"/>
-      <c r="F112" s="63"/>
-      <c r="G112" s="65"/>
-      <c r="H112" s="63"/>
-      <c r="I112" s="65"/>
-      <c r="J112" s="63"/>
-      <c r="K112" s="65"/>
-      <c r="L112" s="63"/>
-      <c r="M112" s="63"/>
-      <c r="N112" s="63"/>
-      <c r="O112" s="63"/>
-      <c r="P112" s="63"/>
-      <c r="Q112" s="63"/>
-      <c r="R112" s="63"/>
-      <c r="S112" s="63"/>
-      <c r="T112" s="63"/>
-      <c r="U112" s="63"/>
-      <c r="V112" s="63"/>
-      <c r="W112" s="63"/>
-      <c r="X112" s="63"/>
-      <c r="Y112" s="63"/>
-      <c r="Z112" s="63"/>
-      <c r="AA112" s="63"/>
-      <c r="AB112" s="63"/>
-    </row>
-    <row r="113" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B113" s="65"/>
-      <c r="C113" s="65"/>
-      <c r="D113" s="65"/>
-      <c r="E113" s="66"/>
-      <c r="F113" s="63"/>
-      <c r="G113" s="65"/>
-      <c r="H113" s="63"/>
-      <c r="I113" s="65"/>
-      <c r="J113" s="63"/>
-      <c r="K113" s="65"/>
-      <c r="L113" s="63"/>
+      <c r="A112" s="64"/>
+      <c r="B112" s="64"/>
+      <c r="C112" s="64"/>
+      <c r="D112" s="64"/>
+      <c r="E112" s="65"/>
+      <c r="F112" s="62"/>
+      <c r="G112" s="64"/>
+      <c r="H112" s="62"/>
+      <c r="I112" s="64"/>
+      <c r="J112" s="62"/>
+      <c r="K112" s="64"/>
+      <c r="L112" s="62"/>
+      <c r="M112" s="62"/>
+      <c r="N112" s="62"/>
+      <c r="O112" s="62"/>
+      <c r="P112" s="62"/>
+      <c r="Q112" s="62"/>
+      <c r="R112" s="62"/>
+      <c r="S112" s="62"/>
+      <c r="T112" s="62"/>
+      <c r="U112" s="62"/>
+      <c r="V112" s="62"/>
+      <c r="W112" s="62"/>
+      <c r="X112" s="62"/>
+      <c r="Y112" s="62"/>
+      <c r="Z112" s="62"/>
+      <c r="AA112" s="62"/>
+      <c r="AB112" s="62"/>
+    </row>
+    <row r="113" spans="2:28" x14ac:dyDescent="0.15">
+      <c r="B113" s="64"/>
+      <c r="C113" s="64"/>
+      <c r="D113" s="64"/>
+      <c r="E113" s="65"/>
+      <c r="F113" s="62"/>
+      <c r="G113" s="64"/>
+      <c r="H113" s="62"/>
+      <c r="I113" s="64"/>
+      <c r="J113" s="62"/>
+      <c r="K113" s="64"/>
+      <c r="L113" s="62"/>
+      <c r="M113" s="62"/>
+      <c r="N113" s="62"/>
+      <c r="O113" s="62"/>
+      <c r="P113" s="62"/>
+      <c r="Q113" s="62"/>
+      <c r="R113" s="62"/>
+      <c r="S113" s="62"/>
+      <c r="T113" s="62"/>
+      <c r="U113" s="62"/>
+      <c r="V113" s="62"/>
+      <c r="W113" s="62"/>
+      <c r="X113" s="62"/>
+      <c r="Y113" s="62"/>
+      <c r="Z113" s="62"/>
+      <c r="AA113" s="62"/>
+      <c r="AB113" s="62"/>
+    </row>
+    <row r="114" spans="2:28" x14ac:dyDescent="0.15">
+      <c r="B114" s="64"/>
+      <c r="C114" s="64"/>
+      <c r="D114" s="64"/>
+      <c r="E114" s="65"/>
+      <c r="F114" s="62"/>
+      <c r="G114" s="64"/>
+      <c r="H114" s="62"/>
+      <c r="I114" s="64"/>
+      <c r="J114" s="62"/>
+      <c r="K114" s="64"/>
+      <c r="L114" s="62"/>
+      <c r="M114" s="62"/>
+      <c r="N114" s="62"/>
+      <c r="O114" s="62"/>
+      <c r="P114" s="62"/>
+      <c r="Q114" s="62"/>
+      <c r="R114" s="62"/>
+      <c r="S114" s="62"/>
+      <c r="T114" s="62"/>
+      <c r="U114" s="62"/>
+      <c r="V114" s="62"/>
+      <c r="W114" s="62"/>
+      <c r="X114" s="62"/>
+      <c r="Y114" s="62"/>
+      <c r="Z114" s="62"/>
+      <c r="AA114" s="62"/>
+      <c r="AB114" s="62"/>
+    </row>
+    <row r="115" spans="2:28" x14ac:dyDescent="0.15">
+      <c r="B115" s="64"/>
+      <c r="C115" s="64"/>
+      <c r="D115" s="64"/>
+      <c r="E115" s="65"/>
+      <c r="F115" s="62"/>
+      <c r="G115" s="64"/>
+      <c r="H115" s="62"/>
+      <c r="I115" s="64"/>
+      <c r="J115" s="62"/>
+      <c r="K115" s="64"/>
+      <c r="L115" s="62"/>
+      <c r="M115" s="62"/>
+      <c r="N115" s="62"/>
+      <c r="O115" s="62"/>
+      <c r="P115" s="62"/>
+      <c r="Q115" s="62"/>
+      <c r="R115" s="62"/>
+      <c r="S115" s="62"/>
+      <c r="T115" s="62"/>
+      <c r="U115" s="62"/>
+      <c r="V115" s="62"/>
+      <c r="W115" s="62"/>
+      <c r="X115" s="62"/>
+      <c r="Y115" s="62"/>
+      <c r="Z115" s="62"/>
+      <c r="AA115" s="62"/>
+      <c r="AB115" s="62"/>
+    </row>
+    <row r="116" spans="2:28" x14ac:dyDescent="0.15">
+      <c r="B116" s="64"/>
+      <c r="C116" s="64"/>
+      <c r="D116" s="64"/>
+      <c r="E116" s="65"/>
+      <c r="F116" s="62"/>
+      <c r="G116" s="64"/>
+      <c r="H116" s="62"/>
+      <c r="I116" s="64"/>
+      <c r="J116" s="62"/>
+      <c r="K116" s="64"/>
+      <c r="L116" s="62"/>
+      <c r="M116" s="62"/>
+      <c r="N116" s="62"/>
+      <c r="O116" s="62"/>
+      <c r="P116" s="62"/>
+      <c r="Q116" s="62"/>
+      <c r="R116" s="62"/>
+      <c r="S116" s="62"/>
+      <c r="T116" s="62"/>
+      <c r="U116" s="62"/>
+      <c r="V116" s="62"/>
+      <c r="W116" s="62"/>
+      <c r="X116" s="62"/>
+      <c r="Y116" s="62"/>
+      <c r="Z116" s="62"/>
+      <c r="AA116" s="62"/>
+      <c r="AB116" s="62"/>
+    </row>
+    <row r="117" spans="2:28" x14ac:dyDescent="0.15">
+      <c r="B117" s="64"/>
+      <c r="C117" s="64"/>
+      <c r="D117" s="64"/>
+      <c r="E117" s="65"/>
+      <c r="F117" s="62"/>
+      <c r="G117" s="64"/>
+      <c r="H117" s="62"/>
+      <c r="I117" s="64"/>
+      <c r="J117" s="62"/>
+      <c r="K117" s="64"/>
+      <c r="L117" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="E97:G97"/>
-    <mergeCell ref="F99:G99"/>
+    <mergeCell ref="E102:G102"/>
+    <mergeCell ref="F103:G103"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.39370078740157483" header="0" footer="0"/>
@@ -4484,8 +4581,8 @@
     <brk id="20" max="11" man="1"/>
     <brk id="33" max="11" man="1"/>
     <brk id="55" max="11" man="1"/>
-    <brk id="70" max="11" man="1"/>
-    <brk id="82" max="11" man="1"/>
+    <brk id="75" max="11" man="1"/>
+    <brk id="87" max="11" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>